<commit_message>
Atualizacao da tabela de materiais e custos/pesos
</commit_message>
<xml_diff>
--- a/Producao/Combate_1kg/materiais.xlsx
+++ b/Producao/Combate_1kg/materiais.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\UnB\Titans\Titans\Producao\Combate_1kg\moledo1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\UnB\Titans\Titans\Producao\Combate_1kg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Rodas</t>
   </si>
@@ -87,6 +87,45 @@
   </si>
   <si>
     <t>https://produto.mercadolivre.com.br/MLB-805964730-esc-hk-50a-4a-ubec-_JM</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>lateral</t>
+  </si>
+  <si>
+    <t>arma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eixo </t>
+  </si>
+  <si>
+    <t>polia</t>
+  </si>
+  <si>
+    <t>MODELO3</t>
+  </si>
+  <si>
+    <t>rolamento</t>
+  </si>
+  <si>
+    <t>MODELO2</t>
+  </si>
+  <si>
+    <t>poliacetal</t>
+  </si>
+  <si>
+    <t>aço</t>
+  </si>
+  <si>
+    <t>tampa</t>
+  </si>
+  <si>
+    <t>(al)</t>
+  </si>
+  <si>
+    <t>mancal</t>
   </si>
 </sst>
 </file>
@@ -94,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -143,7 +182,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7573B177-82BE-4856-BCD8-CE14C405169B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,6 +733,156 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>154</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>71</v>
+      </c>
+      <c r="F16">
+        <v>135</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <f>SUM(B13:B24)</f>
+        <v>1212</v>
+      </c>
+      <c r="E19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>154</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>34</v>
+      </c>
+      <c r="G22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23">
+        <v>34</v>
+      </c>
+      <c r="G23">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f>SUM(B13,E15:E23)</f>
+        <v>1372</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B9">
     <sortCondition ref="A2"/>

</xml_diff>